<commit_message>
adding schedule of this week
</commit_message>
<xml_diff>
--- a/MehdiSchedule.xlsx
+++ b/MehdiSchedule.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="23040" windowHeight="9180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
-    <sheet name="Result" sheetId="2" r:id="rId2"/>
-    <sheet name="Deutsch" sheetId="3" r:id="rId3"/>
+    <sheet name="Estimation" sheetId="4" r:id="rId2"/>
+    <sheet name="Result" sheetId="2" r:id="rId3"/>
+    <sheet name="Deutsch" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>Visual Studio Code</t>
   </si>
@@ -40,9 +41,6 @@
     <t>Microservices</t>
   </si>
   <si>
-    <t>OOP</t>
-  </si>
-  <si>
     <t>SOLID</t>
   </si>
   <si>
@@ -260,13 +258,40 @@
   </si>
   <si>
     <t>Studing the books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVC net  code </t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>12.7.2019</t>
+  </si>
+  <si>
+    <t>complation of S of SOLID</t>
+  </si>
+  <si>
+    <t>End of lesson 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 hours </t>
+  </si>
+  <si>
+    <t>review 1 of 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S of SOLID </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +331,15 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +354,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -349,12 +386,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -369,8 +407,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1883,302 +1923,304 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="M1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
@@ -2872,6 +2914,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
@@ -3147,7 +3272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3163,18 +3288,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add deutsch studing time
</commit_message>
<xml_diff>
--- a/MehdiSchedule.xlsx
+++ b/MehdiSchedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -651,7 +650,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -870,7 +869,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1913,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2045,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
@@ -3162,7 +3160,7 @@
       </c>
       <c r="D2">
         <f>SUM(Scheduling!E:E,Scheduling!E1)</f>
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E2">
         <f>SUM(Scheduling!F:F,Scheduling!F1)</f>

</xml_diff>

<commit_message>
mehdi update 12.8.2019 times
</commit_message>
<xml_diff>
--- a/MehdiSchedule.xlsx
+++ b/MehdiSchedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,6 @@
     <t>میان</t>
   </si>
   <si>
-    <t>Git</t>
-  </si>
-  <si>
     <t>Design Pattern</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>portofilo</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1912,7 +1912,7 @@
   <dimension ref="A1:AG269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,10 +2034,13 @@
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -2047,50 +2050,62 @@
       <c r="E5" s="3">
         <v>90</v>
       </c>
+      <c r="F5" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="F7" s="3">
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>72</v>
+      <c r="A8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="3">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
@@ -2225,7 +2240,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -2936,13 +2951,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2950,21 +2965,21 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2972,32 +2987,32 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3164,7 +3179,7 @@
       </c>
       <c r="E2">
         <f>SUM(Scheduling!F:F,Scheduling!F1)</f>
-        <v>0</v>
+        <v>370</v>
       </c>
       <c r="F2">
         <f>SUM(Scheduling!G:G,Scheduling!G1)</f>

</xml_diff>